<commit_message>
majur functinal changes 10.10.25
</commit_message>
<xml_diff>
--- a/data/last_uploaded.xlsx
+++ b/data/last_uploaded.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,20 +460,25 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Invoice Value</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Due</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Ageing (Days)</t>
         </is>
@@ -494,16 +499,21 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
         <v>53140</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
         <v>53140</v>
       </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -524,16 +534,21 @@
           <t>S2/25-26/ES/002</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
         <v>35621</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
       <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
         <v>35621</v>
       </c>
-      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -554,16 +569,21 @@
           <t>S2/25-26/ES/003</t>
         </is>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
         <v>21365</v>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
       <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>21365</v>
       </c>
-      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -584,16 +604,21 @@
           <t>S2/25-26/ES/004</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
         <v>29367</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
       <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>29367</v>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -614,16 +639,21 @@
           <t>S2/25-26/ES/005</t>
         </is>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>6909</v>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
       <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>6909</v>
       </c>
-      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -644,16 +674,21 @@
           <t>S2/25-26/ES/006</t>
         </is>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
         <v>1201</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
       <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>1201</v>
       </c>
-      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -674,16 +709,21 @@
           <t>S2/25-26/ES/007</t>
         </is>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>6696</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
       <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>6696</v>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -704,16 +744,21 @@
           <t>S2/25-26/ES/008</t>
         </is>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>33883</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
       <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>33883</v>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -734,16 +779,21 @@
           <t>S2/25-26/ES/009</t>
         </is>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>19589</v>
       </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
       <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
         <v>19589</v>
       </c>
-      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -764,16 +814,21 @@
           <t>S2/25-26/ES/010</t>
         </is>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>22832</v>
       </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
       <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
         <v>22832</v>
       </c>
-      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -794,16 +849,21 @@
           <t>S2/25-26/ES/011</t>
         </is>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>179</v>
       </c>
-      <c r="F12" t="n">
-        <v>0</v>
-      </c>
       <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
         <v>179</v>
       </c>
-      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -824,16 +884,21 @@
           <t>S2/25-26/ES/013</t>
         </is>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>26178</v>
       </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
       <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
         <v>26178</v>
       </c>
-      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -854,16 +919,21 @@
           <t>S2/25-26/ES/014</t>
         </is>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>30515</v>
       </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
         <v>30515</v>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -884,16 +954,21 @@
           <t>S2/25-26/ES/015</t>
         </is>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>28577</v>
       </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
       <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
         <v>28577</v>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -914,16 +989,21 @@
           <t>S2/25-26/ES/016</t>
         </is>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
         <v>1220</v>
       </c>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
       <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
         <v>1220</v>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -944,16 +1024,21 @@
           <t>S2/25-26/ES/017</t>
         </is>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
         <v>7563</v>
       </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
       <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
         <v>7563</v>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -974,16 +1059,21 @@
           <t>S2/25-26/ES/018</t>
         </is>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
         <v>8866</v>
       </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
       <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>8866</v>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1004,16 +1094,21 @@
           <t>S2/25-26/ES/019</t>
         </is>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>39998</v>
       </c>
-      <c r="F19" t="n">
-        <v>0</v>
-      </c>
       <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
         <v>39998</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1034,16 +1129,21 @@
           <t>S2/25-26/ES/020</t>
         </is>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
         <v>14145</v>
       </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
       <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
         <v>14145</v>
       </c>
-      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1064,16 +1164,21 @@
           <t>S2/25-26/ES/021</t>
         </is>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
         <v>9583</v>
       </c>
-      <c r="F21" t="n">
-        <v>0</v>
-      </c>
       <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
         <v>9583</v>
       </c>
-      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1094,16 +1199,21 @@
           <t>S2/25-26/ES/022</t>
         </is>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
         <v>33787</v>
       </c>
-      <c r="F22" t="n">
-        <v>0</v>
-      </c>
       <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
         <v>33787</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1124,16 +1234,21 @@
           <t>S2/25-26/ES/023</t>
         </is>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
         <v>665</v>
       </c>
-      <c r="F23" t="n">
-        <v>0</v>
-      </c>
       <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
         <v>665</v>
       </c>
-      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1154,16 +1269,21 @@
           <t>S2/25-26/ES/025</t>
         </is>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
         <v>19797</v>
       </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
       <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
         <v>19797</v>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1184,16 +1304,21 @@
           <t>S2/25-26/ES/026</t>
         </is>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
         <v>22702</v>
       </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
       <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
         <v>22702</v>
       </c>
-      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1214,16 +1339,21 @@
           <t>S2/25-26/ES/027</t>
         </is>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
         <v>24756</v>
       </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
       <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
         <v>24756</v>
       </c>
-      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1244,16 +1374,21 @@
           <t>S2/25-26/ES/028</t>
         </is>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
         <v>3425</v>
       </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
       <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
         <v>3425</v>
       </c>
-      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1274,16 +1409,21 @@
           <t>S2/25-26/ES/029</t>
         </is>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
         <v>17213</v>
       </c>
-      <c r="F28" t="n">
-        <v>0</v>
-      </c>
       <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
         <v>17213</v>
       </c>
-      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1304,16 +1444,21 @@
           <t>S2/25-26/ES/030</t>
         </is>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
         <v>17901</v>
       </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
       <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
         <v>17901</v>
       </c>
-      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1334,16 +1479,21 @@
           <t>S2/25-26/ES/031</t>
         </is>
       </c>
-      <c r="E30" t="n">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
         <v>40284</v>
       </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
       <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
         <v>40284</v>
       </c>
-      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1364,16 +1514,21 @@
           <t>S2/25-26/ES/032</t>
         </is>
       </c>
-      <c r="E31" t="n">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
         <v>34528</v>
       </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
       <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
         <v>34528</v>
       </c>
-      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1394,16 +1549,21 @@
           <t>S2/25-26/ES/033</t>
         </is>
       </c>
-      <c r="E32" t="n">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
         <v>1105</v>
       </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
       <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
         <v>1105</v>
       </c>
-      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1424,16 +1584,21 @@
           <t>S2/25-26/ES/036</t>
         </is>
       </c>
-      <c r="E33" t="n">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
         <v>7891</v>
       </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
       <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
         <v>7891</v>
       </c>
-      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1454,16 +1619,21 @@
           <t>S2/25-26/ES/037</t>
         </is>
       </c>
-      <c r="E34" t="n">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
         <v>23002</v>
       </c>
-      <c r="F34" t="n">
-        <v>0</v>
-      </c>
       <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
         <v>23002</v>
       </c>
-      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1484,16 +1654,21 @@
           <t>S2/25-26/ES/038</t>
         </is>
       </c>
-      <c r="E35" t="n">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
         <v>22623</v>
       </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
       <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
         <v>22623</v>
       </c>
-      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1514,16 +1689,21 @@
           <t>S2/25-26/ES/039</t>
         </is>
       </c>
-      <c r="E36" t="n">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
         <v>7483</v>
       </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
       <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
         <v>7483</v>
       </c>
-      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1544,16 +1724,21 @@
           <t>S2/25-26/ES/040</t>
         </is>
       </c>
-      <c r="E37" t="n">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
         <v>12244</v>
       </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
       <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
         <v>12244</v>
       </c>
-      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1574,16 +1759,21 @@
           <t>S2/25-26/ES/041</t>
         </is>
       </c>
-      <c r="E38" t="n">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
         <v>50031</v>
       </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
       <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
         <v>50031</v>
       </c>
-      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1604,16 +1794,21 @@
           <t>S2/25-26/ES/042</t>
         </is>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
         <v>2261</v>
       </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
       <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
         <v>2261</v>
       </c>
-      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1634,16 +1829,21 @@
           <t>S2/25-26/ES/045</t>
         </is>
       </c>
-      <c r="E40" t="n">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
         <v>8137</v>
       </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
       <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
         <v>8137</v>
       </c>
-      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1664,16 +1864,21 @@
           <t>S2/25-26/ES/046</t>
         </is>
       </c>
-      <c r="E41" t="n">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
         <v>29890</v>
       </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
       <c r="G41" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" t="n">
         <v>29890</v>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1694,16 +1899,21 @@
           <t>S2/25-26/ES/047</t>
         </is>
       </c>
-      <c r="E42" t="n">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
         <v>10394</v>
       </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
       <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
         <v>10394</v>
       </c>
-      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1724,16 +1934,21 @@
           <t>S2/25-26/ES/048</t>
         </is>
       </c>
-      <c r="E43" t="n">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
         <v>19659</v>
       </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
       <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
         <v>19659</v>
       </c>
-      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1754,16 +1969,21 @@
           <t>S2/25-26/ES/049</t>
         </is>
       </c>
-      <c r="E44" t="n">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
         <v>60684</v>
       </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
       <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
         <v>60684</v>
       </c>
-      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1784,16 +2004,21 @@
           <t>S2/25-26/ES/050</t>
         </is>
       </c>
-      <c r="E45" t="n">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
         <v>8123</v>
       </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
       <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
         <v>8123</v>
       </c>
-      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1814,16 +2039,21 @@
           <t>S2/25-26/ES/051</t>
         </is>
       </c>
-      <c r="E46" t="n">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
         <v>30737</v>
       </c>
-      <c r="F46" t="n">
-        <v>0</v>
-      </c>
       <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
         <v>30737</v>
       </c>
-      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1844,16 +2074,21 @@
           <t>S2/25-26/ES/052</t>
         </is>
       </c>
-      <c r="E47" t="n">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
         <v>21548</v>
       </c>
-      <c r="F47" t="n">
-        <v>0</v>
-      </c>
       <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
         <v>21548</v>
       </c>
-      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1874,16 +2109,21 @@
           <t>S2/25-26/ES/053</t>
         </is>
       </c>
-      <c r="E48" t="n">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
         <v>59056</v>
       </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
       <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
         <v>59056</v>
       </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1904,16 +2144,21 @@
           <t>S2/24-25/LS/002</t>
         </is>
       </c>
-      <c r="E49" t="n">
-        <v>118000</v>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F49" t="n">
         <v>118000</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
-      </c>
-      <c r="H49" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1934,16 +2179,21 @@
           <t>S2/24-25/LS/003</t>
         </is>
       </c>
-      <c r="E50" t="n">
-        <v>54312</v>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F50" t="n">
         <v>54312</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
-      </c>
-      <c r="H50" t="inlineStr"/>
+        <v>54312</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1964,16 +2214,21 @@
           <t>S2/24-25/LS/005</t>
         </is>
       </c>
-      <c r="E51" t="n">
-        <v>118000</v>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F51" t="n">
         <v>118000</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
-      </c>
-      <c r="H51" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1994,16 +2249,21 @@
           <t>S2/24-25/LS/006</t>
         </is>
       </c>
-      <c r="E52" t="n">
-        <v>118000</v>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F52" t="n">
         <v>118000</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H52" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2024,16 +2284,21 @@
           <t>S2/24-25/LS/010</t>
         </is>
       </c>
-      <c r="E53" t="n">
-        <v>118000</v>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F53" t="n">
         <v>118000</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2054,16 +2319,21 @@
           <t>S2/24-25/LS/011</t>
         </is>
       </c>
-      <c r="E54" t="n">
-        <v>118000</v>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F54" t="n">
         <v>118000</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2084,16 +2354,21 @@
           <t>S2/24-25/LS/012</t>
         </is>
       </c>
-      <c r="E55" t="n">
-        <v>118000</v>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F55" t="n">
         <v>118000</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2114,16 +2389,21 @@
           <t>S2/24-25/LS/013</t>
         </is>
       </c>
-      <c r="E56" t="n">
-        <v>118000</v>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F56" t="n">
         <v>118000</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2144,16 +2424,21 @@
           <t>S2/24-25/LS/016</t>
         </is>
       </c>
-      <c r="E57" t="n">
-        <v>118000</v>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F57" t="n">
         <v>118000</v>
       </c>
       <c r="G57" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2174,16 +2459,21 @@
           <t>S2/24-25/LS/017</t>
         </is>
       </c>
-      <c r="E58" t="n">
-        <v>118000</v>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F58" t="n">
         <v>118000</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2204,16 +2494,21 @@
           <t>S2/24-25/LS/020</t>
         </is>
       </c>
-      <c r="E59" t="n">
-        <v>236000</v>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F59" t="n">
         <v>236000</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="inlineStr"/>
+        <v>236000</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2234,16 +2529,21 @@
           <t>S2/24-25/LS/023</t>
         </is>
       </c>
-      <c r="E60" t="n">
-        <v>192734</v>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F60" t="n">
         <v>192734</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" t="inlineStr"/>
+        <v>192734</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2264,16 +2564,21 @@
           <t>S2/24-25/LS/023</t>
         </is>
       </c>
-      <c r="E61" t="n">
-        <v>118000</v>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F61" t="n">
         <v>118000</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2294,16 +2599,21 @@
           <t>S2/24-25/LS/027</t>
         </is>
       </c>
-      <c r="E62" t="n">
-        <v>118000</v>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F62" t="n">
         <v>118000</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2324,16 +2634,21 @@
           <t>S2/24-25/LS/029</t>
         </is>
       </c>
-      <c r="E63" t="n">
-        <v>118000</v>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F63" t="n">
         <v>118000</v>
       </c>
       <c r="G63" t="n">
-        <v>0</v>
-      </c>
-      <c r="H63" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2354,16 +2669,21 @@
           <t>S2/24-25/LS/031</t>
         </is>
       </c>
-      <c r="E64" t="n">
-        <v>118000</v>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F64" t="n">
         <v>118000</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
-      </c>
-      <c r="H64" t="inlineStr"/>
+        <v>118000</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2384,16 +2704,21 @@
           <t>S2/25-26/LS/001</t>
         </is>
       </c>
-      <c r="E65" t="n">
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
         <v>118000</v>
       </c>
-      <c r="F65" t="n">
-        <v>0</v>
-      </c>
       <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
         <v>118000</v>
       </c>
-      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2414,16 +2739,21 @@
           <t>S2/24-25/LS/001</t>
         </is>
       </c>
-      <c r="E66" t="n">
-        <v>177000</v>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F66" t="n">
         <v>177000</v>
       </c>
       <c r="G66" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" t="inlineStr"/>
+        <v>177000</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2444,16 +2774,21 @@
           <t>S2/24-25/LS/004</t>
         </is>
       </c>
-      <c r="E67" t="n">
-        <v>177000</v>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F67" t="n">
         <v>177000</v>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
-      </c>
-      <c r="H67" t="inlineStr"/>
+        <v>177000</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2474,16 +2809,21 @@
           <t>S2/24-25/LS/007</t>
         </is>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
         <v>786145.5</v>
       </c>
-      <c r="F68" t="n">
-        <v>0</v>
-      </c>
       <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" t="n">
         <v>786145.5</v>
       </c>
-      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2504,16 +2844,21 @@
           <t>S2/24-25/LS/008</t>
         </is>
       </c>
-      <c r="E69" t="n">
-        <v>184080</v>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F69" t="n">
         <v>184080</v>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
-      </c>
-      <c r="H69" t="inlineStr"/>
+        <v>184080</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2534,16 +2879,21 @@
           <t>S2/24-25/LS/009</t>
         </is>
       </c>
-      <c r="E70" t="n">
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
         <v>607464</v>
       </c>
-      <c r="F70" t="n">
-        <v>0</v>
-      </c>
       <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
         <v>607464</v>
       </c>
-      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2564,16 +2914,21 @@
           <t>S2/24-25/LS/015</t>
         </is>
       </c>
-      <c r="E71" t="n">
-        <v>177000</v>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F71" t="n">
         <v>177000</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
-      </c>
-      <c r="H71" t="inlineStr"/>
+        <v>177000</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2594,16 +2949,21 @@
           <t>S2/24-25/LS/019</t>
         </is>
       </c>
-      <c r="E72" t="n">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
         <v>1068456.96</v>
       </c>
-      <c r="F72" t="n">
-        <v>0</v>
-      </c>
       <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
         <v>1068456.96</v>
       </c>
-      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2624,16 +2984,21 @@
           <t>S2/24-25/LS/022</t>
         </is>
       </c>
-      <c r="E73" t="n">
-        <v>354000</v>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F73" t="n">
         <v>354000</v>
       </c>
       <c r="G73" t="n">
-        <v>0</v>
-      </c>
-      <c r="H73" t="inlineStr"/>
+        <v>354000</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2654,16 +3019,21 @@
           <t>S2/24-25/LS/024</t>
         </is>
       </c>
-      <c r="E74" t="n">
-        <v>177000</v>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F74" t="n">
         <v>177000</v>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
-      </c>
-      <c r="H74" t="inlineStr"/>
+        <v>177000</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2684,16 +3054,21 @@
           <t>S2/24-25/LS/026</t>
         </is>
       </c>
-      <c r="E75" t="n">
-        <v>177000</v>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F75" t="n">
         <v>177000</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
-      </c>
-      <c r="H75" t="inlineStr"/>
+        <v>177000</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2714,16 +3089,21 @@
           <t>S2/24-25/LS/028</t>
         </is>
       </c>
-      <c r="E76" t="n">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
         <v>177000</v>
       </c>
-      <c r="F76" t="n">
-        <v>0</v>
-      </c>
       <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" t="n">
         <v>177000</v>
       </c>
-      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2744,16 +3124,21 @@
           <t>S2/25-26/ES/001</t>
         </is>
       </c>
-      <c r="E77" t="n">
-        <v>23742</v>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F77" t="n">
         <v>23742</v>
       </c>
       <c r="G77" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" t="inlineStr"/>
+        <v>23742</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2774,16 +3159,21 @@
           <t>S2/25-26/ES/043</t>
         </is>
       </c>
-      <c r="E78" t="n">
-        <v>80500</v>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F78" t="n">
         <v>80500</v>
       </c>
       <c r="G78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" t="inlineStr"/>
+        <v>80500</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2804,16 +3194,21 @@
           <t>S2/24-25/LS/030</t>
         </is>
       </c>
-      <c r="E79" t="n">
-        <v>52864</v>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F79" t="n">
         <v>52864</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" t="inlineStr"/>
+        <v>52864</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2834,16 +3229,21 @@
           <t>S2/25-26/LS/002</t>
         </is>
       </c>
-      <c r="E80" t="n">
-        <v>72688</v>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F80" t="n">
         <v>72688</v>
       </c>
       <c r="G80" t="n">
-        <v>0</v>
-      </c>
-      <c r="H80" t="inlineStr"/>
+        <v>72688</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2864,16 +3264,21 @@
           <t>S2/25-26/LS/030</t>
         </is>
       </c>
-      <c r="E81" t="n">
-        <v>161896</v>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
       </c>
       <c r="F81" t="n">
         <v>161896</v>
       </c>
       <c r="G81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H81" t="inlineStr"/>
+        <v>161896</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2894,16 +3299,21 @@
           <t>S2I/25-26/ES/012</t>
         </is>
       </c>
-      <c r="E82" t="n">
-        <v>16272</v>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F82" t="n">
         <v>16272</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
-      </c>
-      <c r="H82" t="inlineStr"/>
+        <v>16272</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2924,16 +3334,21 @@
           <t>S2I/25-26/ES/024</t>
         </is>
       </c>
-      <c r="E83" t="n">
-        <v>21552</v>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F83" t="n">
         <v>21552</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H83" t="inlineStr"/>
+        <v>21552</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2954,16 +3369,21 @@
           <t>S2I/25-26/ES/034</t>
         </is>
       </c>
-      <c r="E84" t="n">
-        <v>22080</v>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F84" t="n">
         <v>22080</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
-      </c>
-      <c r="H84" t="inlineStr"/>
+        <v>22080</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2984,16 +3404,21 @@
           <t>S2I/25-26/ES/035</t>
         </is>
       </c>
-      <c r="E85" t="n">
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
         <v>4294</v>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>4257</v>
       </c>
-      <c r="G85" t="n">
+      <c r="H85" t="n">
         <v>37</v>
       </c>
-      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3014,16 +3439,21 @@
           <t>S2I/25-26/ES/044</t>
         </is>
       </c>
-      <c r="E86" t="n">
-        <v>24048</v>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F86" t="n">
         <v>24048</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
-      </c>
-      <c r="H86" t="inlineStr"/>
+        <v>24048</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3044,16 +3474,21 @@
           <t>S2I/25-26/ES/052</t>
         </is>
       </c>
-      <c r="E87" t="n">
-        <v>26848</v>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F87" t="n">
         <v>26848</v>
       </c>
       <c r="G87" t="n">
-        <v>0</v>
-      </c>
-      <c r="H87" t="inlineStr"/>
+        <v>26848</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3074,16 +3509,21 @@
           <t>S2/25-26/ES/045</t>
         </is>
       </c>
-      <c r="E88" t="n">
-        <v>38300</v>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F88" t="n">
         <v>38300</v>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H88" t="inlineStr"/>
+        <v>38300</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3104,16 +3544,21 @@
           <t>S2/25-26/ES/046</t>
         </is>
       </c>
-      <c r="E89" t="n">
-        <v>38300</v>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
       </c>
       <c r="F89" t="n">
         <v>38300</v>
       </c>
       <c r="G89" t="n">
-        <v>0</v>
-      </c>
-      <c r="H89" t="inlineStr"/>
+        <v>38300</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3134,16 +3579,21 @@
           <t>S2/25-26/LS/003</t>
         </is>
       </c>
-      <c r="E90" t="n">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
         <v>603046</v>
       </c>
-      <c r="F90" t="n">
-        <v>0</v>
-      </c>
       <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" t="n">
         <v>603046</v>
       </c>
-      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3164,16 +3614,21 @@
           <t>S2/25-26/LS/004</t>
         </is>
       </c>
-      <c r="E91" t="n">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
         <v>394852</v>
       </c>
-      <c r="F91" t="n">
-        <v>0</v>
-      </c>
       <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" t="n">
         <v>394852</v>
       </c>
-      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3194,16 +3649,21 @@
           <t>S2/25-26/LS/005</t>
         </is>
       </c>
-      <c r="E92" t="n">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
         <v>355367</v>
       </c>
-      <c r="F92" t="n">
-        <v>0</v>
-      </c>
       <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" t="n">
         <v>355367</v>
       </c>
-      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3224,16 +3684,21 @@
           <t>S2/25-26/LS/006</t>
         </is>
       </c>
-      <c r="E93" t="n">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
         <v>376904</v>
       </c>
-      <c r="F93" t="n">
-        <v>0</v>
-      </c>
       <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
         <v>376904</v>
       </c>
-      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3254,16 +3719,21 @@
           <t>S2/25-26/LS/007</t>
         </is>
       </c>
-      <c r="E94" t="n">
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
         <v>339214</v>
       </c>
-      <c r="F94" t="n">
-        <v>0</v>
-      </c>
       <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" t="n">
         <v>339214</v>
       </c>
-      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3284,16 +3754,21 @@
           <t>S2/25-26/LS/008</t>
         </is>
       </c>
-      <c r="E95" t="n">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
         <v>412799</v>
       </c>
-      <c r="F95" t="n">
-        <v>0</v>
-      </c>
       <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" t="n">
         <v>412799</v>
       </c>
-      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3314,16 +3789,21 @@
           <t>S2/25-26/LS/009</t>
         </is>
       </c>
-      <c r="E96" t="n">
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F96" t="n">
         <v>488180</v>
       </c>
-      <c r="F96" t="n">
-        <v>0</v>
-      </c>
       <c r="G96" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" t="n">
         <v>488180</v>
       </c>
-      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3344,16 +3824,21 @@
           <t>S2/25-26/LS/010</t>
         </is>
       </c>
-      <c r="E97" t="n">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
         <v>341008</v>
       </c>
-      <c r="F97" t="n">
-        <v>0</v>
-      </c>
       <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" t="n">
         <v>341008</v>
       </c>
-      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3374,16 +3859,21 @@
           <t>S2/25-26/LS/011</t>
         </is>
       </c>
-      <c r="E98" t="n">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F98" t="n">
         <v>290755</v>
       </c>
-      <c r="F98" t="n">
-        <v>0</v>
-      </c>
       <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" t="n">
         <v>290755</v>
       </c>
-      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3404,16 +3894,21 @@
           <t>S2/25-26/LS/012</t>
         </is>
       </c>
-      <c r="E99" t="n">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F99" t="n">
         <v>323060</v>
       </c>
-      <c r="F99" t="n">
-        <v>0</v>
-      </c>
       <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" t="n">
         <v>323060</v>
       </c>
-      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3434,16 +3929,21 @@
           <t>S2/25-26/LS/013</t>
         </is>
       </c>
-      <c r="E100" t="n">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F100" t="n">
         <v>250372</v>
       </c>
-      <c r="F100" t="n">
-        <v>0</v>
-      </c>
       <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
         <v>250372</v>
       </c>
-      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3464,16 +3964,21 @@
           <t>S2/25-26/LS/014</t>
         </is>
       </c>
-      <c r="E101" t="n">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F101" t="n">
         <v>341008</v>
       </c>
-      <c r="F101" t="n">
-        <v>0</v>
-      </c>
       <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" t="n">
         <v>341008</v>
       </c>
-      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3494,16 +3999,21 @@
           <t>S2/25-26/LS/015</t>
         </is>
       </c>
-      <c r="E102" t="n">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F102" t="n">
         <v>412799</v>
       </c>
-      <c r="F102" t="n">
-        <v>0</v>
-      </c>
       <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" t="n">
         <v>412799</v>
       </c>
-      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3524,16 +4034,21 @@
           <t>S2/25-26/LS/016</t>
         </is>
       </c>
-      <c r="E103" t="n">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>₹</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
         <v>341008</v>
       </c>
-      <c r="F103" t="n">
-        <v>0</v>
-      </c>
       <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" t="n">
         <v>341008</v>
       </c>
-      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>